<commit_message>
Entorno de test a pytest (iss. #18)
</commit_message>
<xml_diff>
--- a/conta/main/tests/data/plantilla_errores.xlsx
+++ b/conta/main/tests/data/plantilla_errores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\Nextcloud\Programacion\GitHub\contabilidad\conta\main\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E6206E-136F-4A81-8CDF-3585717B8691}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E433742C-840A-4294-A97B-81A1478179A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simple" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>Fecha</t>
   </si>
@@ -219,13 +219,22 @@
     <t>Factura EDP - electricidad</t>
   </si>
   <si>
-    <t>aj</t>
-  </si>
-  <si>
     <t>comida</t>
   </si>
   <si>
     <t>Cenas, pinchos…</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Comida - propina</t>
+  </si>
+  <si>
+    <t>Comida - total</t>
+  </si>
+  <si>
+    <t>gege</t>
   </si>
 </sst>
 </file>
@@ -760,7 +769,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
@@ -776,6 +785,10 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="17" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="17" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="17" fillId="34" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="17" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -828,16 +841,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -857,6 +860,16 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1180,7 +1193,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92DFB669-943E-4FB1-BFE0-6600908D48A8}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="asient">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{92DFB669-943E-4FB1-BFE0-6600908D48A8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="asient">
   <location ref="J3:M5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -1513,20 +1526,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35FB1CE0-CDC9-4398-8590-3A1B4B1E6CD8}" name="Mov_complejo" displayName="Mov_complejo" ref="B3:H9" totalsRowShown="0">
-  <autoFilter ref="B3:H9" xr:uid="{47D0FA3E-EDD9-4A2A-92E8-A35A238EDB76}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35FB1CE0-CDC9-4398-8590-3A1B4B1E6CD8}" name="Mov_complejo" displayName="Mov_complejo" ref="B3:H12" totalsRowShown="0">
+  <autoFilter ref="B3:H12" xr:uid="{47D0FA3E-EDD9-4A2A-92E8-A35A238EDB76}"/>
   <tableColumns count="7">
     <tableColumn id="6" xr3:uid="{9AD972E4-C579-4424-B1C1-7A8548B415A4}" name="id"/>
-    <tableColumn id="1" xr3:uid="{F37AE433-6E34-4726-AC7C-8ED9ECE4E316}" name="Fecha" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{93B832D8-D900-4EA3-971C-04F4F4F73E5E}" name="Descripción" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{365E1047-CFC9-4957-AC96-690DF270BD6C}" name="Debe" dataDxfId="5" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{F37AE433-6E34-4726-AC7C-8ED9ECE4E316}" name="Fecha" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{93B832D8-D900-4EA3-971C-04F4F4F73E5E}" name="Descripción" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{365E1047-CFC9-4957-AC96-690DF270BD6C}" name="Debe" dataDxfId="4" dataCellStyle="Comma">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C8820A2C-D1F4-429F-BEE6-9CFD5D206202}" name="Haber" dataDxfId="4" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{C8820A2C-D1F4-429F-BEE6-9CFD5D206202}" name="Haber" dataDxfId="3" dataCellStyle="Comma">
       <calculatedColumnFormula>0</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A593CEC0-C069-4610-84D5-1989C29A9B0E}" name="Cuenta" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{1BDE309D-E6E3-4D7F-9F73-061A12ACC2FE}" name="Cuenta descr" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{A593CEC0-C069-4610-84D5-1989C29A9B0E}" name="Cuenta" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{1BDE309D-E6E3-4D7F-9F73-061A12ACC2FE}" name="Cuenta descr" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1538,7 +1551,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{447D7112-259D-4C0C-AF28-055C99274BD5}" name="Cuentas" displayName="Cuentas" ref="F4:G17" totalsRowShown="0">
   <autoFilter ref="F4:G17" xr:uid="{6F18564F-6990-4186-B512-9E1C6E9F5F3A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9DE84074-E3ED-46A0-8037-CE36B265F541}" name="Cuenta" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{9DE84074-E3ED-46A0-8037-CE36B265F541}" name="Cuenta" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{C60FC6EA-5DD3-4D2E-A6C5-929976B15FC4}" name="Descripción"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1844,7 +1857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C68A8C-4B2B-40F9-A6AA-47048CD7600B}">
   <dimension ref="B3:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1887,7 +1900,7 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
@@ -2035,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5C23EA-5D97-488D-B298-E89BE659774C}">
-  <dimension ref="B3:P9"/>
+  <dimension ref="B3:P18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2092,9 +2105,6 @@
       <c r="O3" t="s">
         <v>29</v>
       </c>
-      <c r="P3" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -2146,12 +2156,12 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="5" t="str">
+      <c r="G5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="5" t="e">
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
-        <v>Caja</v>
+        <v>#N/A</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>34</v>
@@ -2193,7 +2203,7 @@
         <v>Cenas, pinchos…</v>
       </c>
       <c r="O6" t="str" cm="1">
-        <f t="array" ref="O6:P6">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(P3,Cuentas[Descripción]))))</f>
+        <f t="array" ref="O6:P18">_xlfn._xlws.FILTER(Cuentas[],(ISNUMBER(SEARCH(P3,Cuentas[Descripción]))))</f>
         <v>100</v>
       </c>
       <c r="P6" t="str">
@@ -2213,7 +2223,7 @@
       <c r="E7" s="10">
         <v>150</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="7" t="s">
         <v>13</v>
       </c>
@@ -2221,6 +2231,12 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Cuenta nómina</v>
       </c>
+      <c r="O7" t="str">
+        <v>101</v>
+      </c>
+      <c r="P7" t="str">
+        <v>Tickets restaurant</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8">
@@ -2246,6 +2262,12 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Gas casa</v>
       </c>
+      <c r="O8" t="str">
+        <v>1101</v>
+      </c>
+      <c r="P8" t="str">
+        <v>Cuenta nómina</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9">
@@ -2257,7 +2279,7 @@
       <c r="D9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="2">
         <v>30</v>
       </c>
@@ -2268,10 +2290,155 @@
         <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
         <v>Electricidad casa</v>
       </c>
+      <c r="O9" t="str">
+        <v>1110</v>
+      </c>
+      <c r="P9" t="str">
+        <v>Cuenta ahorro</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="15"/>
+      <c r="C10" s="1">
+        <v>44544</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10">
+        <v>25</v>
+      </c>
+      <c r="F10" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5" t="str">
+        <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
+        <v>Tarjeta Visa</v>
+      </c>
+      <c r="O10" t="str">
+        <v>1200</v>
+      </c>
+      <c r="P10" t="str">
+        <v>Tarjeta Visa</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2</v>
+      </c>
+      <c r="F11" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="5" t="str">
+        <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
+        <v>Caja</v>
+      </c>
+      <c r="O11" t="str">
+        <v>1201</v>
+      </c>
+      <c r="P11" t="str">
+        <v>Tarjeta Amex</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44544</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="10">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>27</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="5" t="str">
+        <f>VLOOKUP(Mov_complejo[[#This Row],[Cuenta]],Cuentas[],2,FALSE)</f>
+        <v>Cenas, pinchos…</v>
+      </c>
+      <c r="O12" t="str">
+        <v>1210</v>
+      </c>
+      <c r="P12" t="str">
+        <v>Tarjeta prepago</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O13" t="str">
+        <v>300</v>
+      </c>
+      <c r="P13" t="str">
+        <v>Comida</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O14" t="str">
+        <v>312</v>
+      </c>
+      <c r="P14" t="str">
+        <v>Cenas, pinchos…</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O15" t="str">
+        <v>324</v>
+      </c>
+      <c r="P15" t="str">
+        <v>Gastos coche</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O16" t="str">
+        <v>15</v>
+      </c>
+      <c r="P16" t="str">
+        <v>Hipoteca</v>
+      </c>
+    </row>
+    <row r="17" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O17" t="str">
+        <v>2001</v>
+      </c>
+      <c r="P17" t="str">
+        <v>Gas casa</v>
+      </c>
+    </row>
+    <row r="18" spans="15:16" x14ac:dyDescent="0.3">
+      <c r="O18" t="str">
+        <v>2000</v>
+      </c>
+      <c r="P18" t="str">
+        <v>Electricidad casa</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="M4:M5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2405,7 +2572,7 @@
         <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>